<commit_message>
March 2023 Release: version 10.0.2
</commit_message>
<xml_diff>
--- a/data/transit_time.xlsx
+++ b/data/transit_time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65925644-AE06-4695-9346-07D202683E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A88C0C-B205-48CB-9B17-100745EA99AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Portugal</t>
   </si>
@@ -71,9 +71,6 @@
     <t>MUAC</t>
   </si>
   <si>
-    <t>Serbia</t>
-  </si>
-  <si>
     <t>Croatia</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Estonia</t>
   </si>
   <si>
-    <t>UK</t>
-  </si>
-  <si>
     <t>Denmark</t>
   </si>
   <si>
@@ -122,12 +116,6 @@
     <t>Albania</t>
   </si>
   <si>
-    <t>Slovak Republic</t>
-  </si>
-  <si>
-    <t>Moldova</t>
-  </si>
-  <si>
     <t>Switzerland</t>
   </si>
   <si>
@@ -143,23 +131,159 @@
     <t>Belgium</t>
   </si>
   <si>
-    <t>Weighted average</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
-    <t>time</t>
+    <t>ansp</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>Albcontrol</t>
+  </si>
+  <si>
+    <t>ANS CR</t>
+  </si>
+  <si>
+    <t>ANS Finland</t>
+  </si>
+  <si>
+    <t>ARMATS</t>
+  </si>
+  <si>
+    <t>Austro Control</t>
+  </si>
+  <si>
+    <t>AVINOR (Continental)</t>
+  </si>
+  <si>
+    <t>BULATSA</t>
+  </si>
+  <si>
+    <t>Croatia Control</t>
+  </si>
+  <si>
+    <t>DCAC Cyprus</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>DHMI</t>
+  </si>
+  <si>
+    <t>DSNA</t>
+  </si>
+  <si>
+    <t>EANS</t>
+  </si>
+  <si>
+    <t>ENAIRE</t>
+  </si>
+  <si>
+    <t>ENAV</t>
+  </si>
+  <si>
+    <t>HCAA</t>
+  </si>
+  <si>
+    <t>HungaroControl</t>
+  </si>
+  <si>
+    <t>IAA</t>
+  </si>
+  <si>
+    <t>LFV</t>
+  </si>
+  <si>
+    <t>LGS</t>
+  </si>
+  <si>
+    <t>LPS</t>
+  </si>
+  <si>
+    <t>LVNL</t>
+  </si>
+  <si>
+    <t>MATS</t>
+  </si>
+  <si>
+    <t>M-NAV</t>
+  </si>
+  <si>
+    <t>MOLDATSA</t>
+  </si>
+  <si>
+    <t>NATS (Continental)</t>
+  </si>
+  <si>
+    <t>NAV Portugal (Continental)</t>
+  </si>
+  <si>
+    <t>NAVIAIR</t>
+  </si>
+  <si>
+    <t>Oro Navigacija</t>
+  </si>
+  <si>
+    <t>PANSA</t>
+  </si>
+  <si>
+    <t>ROMATSA</t>
+  </si>
+  <si>
+    <t>SAKAERONAVIGATSIA</t>
+  </si>
+  <si>
+    <t>skeyes</t>
+  </si>
+  <si>
+    <t>Skyguide</t>
+  </si>
+  <si>
+    <t>Slovenia Control</t>
+  </si>
+  <si>
+    <t>SMATSA</t>
+  </si>
+  <si>
+    <t>UkSATSE</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Republic of Moldova</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Serbia &amp; Montenegro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,8 +309,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,7 +618,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,320 +626,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" t="s">
         <v>28</v>
       </c>
-      <c r="B2">
+      <c r="C37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28">
+      <c r="C39">
         <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -827,18 +1074,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1065,6 +1312,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFC75A0-E02F-4958-BA20-E0643BE00BFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C121DFFC-1C78-46A8-AC2D-286473FD2932}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1077,14 +1332,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="c78a888a-83d8-49bb-8890-6eb97e8a3c0e"/>
     <ds:schemaRef ds:uri="841a37d2-6ac6-4cb8-8211-c8824e7b4dcd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFC75A0-E02F-4958-BA20-E0643BE00BFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>